<commit_message>
fix missing eService attribute for first user
</commit_message>
<xml_diff>
--- a/wallet-enterprise-configurations/issuer/dataset/por-dataset.xlsx
+++ b/wallet-enterprise-configurations/issuer/dataset/por-dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t xml:space="preserve">pid_id</t>
   </si>
@@ -73,6 +73,9 @@
     <t xml:space="preserve">2028-01-01T00:00:00Z</t>
   </si>
   <si>
+    <t xml:space="preserve">Registration of a business</t>
+  </si>
+  <si>
     <t xml:space="preserve">PID:00001</t>
   </si>
   <si>
@@ -98,9 +101,6 @@
   </si>
   <si>
     <t xml:space="preserve">2029-01-01T00:00:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registration of a business</t>
   </si>
   <si>
     <t xml:space="preserve">PID:00002</t>
@@ -205,14 +205,14 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
+      <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+      <left/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
@@ -246,52 +246,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="15" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -315,8 +319,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF7F7F7"/>
-          <bgColor rgb="FF272727"/>
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -345,138 +349,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="1" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="8" t="n">
+      <c r="K2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="10" t="n">
         <v>33161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="8" t="n">
+      <c r="L3" s="10" t="n">
         <v>33161</v>
       </c>
     </row>

</xml_diff>